<commit_message>
Added suspension measurements file
</commit_message>
<xml_diff>
--- a/param.xlsx
+++ b/param.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Robotics\vroomvroom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{764E8BC3-35B5-4887-9168-3EC0B915C417}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3CB272C-938C-4741-BE2F-D108034ECE9E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="12735" xr2:uid="{9F73D4E3-3970-4AB3-9609-1314AE1B41B8}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>Name</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>relaxedSpringLength</t>
+  </si>
+  <si>
+    <t>suspensionAngle</t>
+  </si>
+  <si>
+    <t>deg</t>
   </si>
 </sst>
 </file>
@@ -418,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEF2AB97-6B65-40C9-BCAB-8EDE625EC945}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,6 +526,17 @@
         <v>9</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>45</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>